<commit_message>
No funciona el control de volumen : (
</commit_message>
<xml_diff>
--- a/calculo volumen.xlsx
+++ b/calculo volumen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrenbg1\Desktop\DSED-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37780555-83FA-4267-A989-C179773155C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E99814B-B93F-479E-82B5-71F841410EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7B6F0A07-A816-4495-8DC4-CF44D00883B9}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" xr2:uid="{7B6F0A07-A816-4495-8DC4-CF44D00883B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -410,12 +410,15 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+      <selection activeCell="D2" sqref="D2:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="21.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -429,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -438,19 +441,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>ROUND(B2*2^4, 0)</f>
+        <f>ROUND(B2*2^7, 0)</f>
         <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>DEC2BIN(C2, 8)</f>
-        <v>00000000</v>
+        <f>_xlfn.CONCAT(DEC2BIN(C2/256,8), DEC2BIN(MOD(C2, 256),8))</f>
+        <v>0000000000000000</v>
       </c>
       <c r="E2" t="str">
         <f>_xlfn.CONCAT("s",A2)</f>
         <v>s0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -459,19 +462,19 @@
         <v>3.5802340673177814E-2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="1">ROUND(B3*2^4, 0)</f>
-        <v>1</v>
+        <f t="shared" ref="C3:C22" si="1">ROUND(B3*2^7, 0)</f>
+        <v>5</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D22" si="2">DEC2BIN(C3, 8)</f>
-        <v>00000001</v>
+        <f t="shared" ref="D3:D22" si="2">_xlfn.CONCAT(DEC2BIN(C3/256,8), DEC2BIN(MOD(C3, 256),8))</f>
+        <v>0000000000000101</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E22" si="3">_xlfn.CONCAT("s",A3)</f>
         <v>s1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -482,18 +485,18 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>00000001</v>
+        <v>0000000000001010</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
         <v>s2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:A22" si="4">A4+1</f>
         <v>3</v>
@@ -504,18 +507,18 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
-        <v>00000010</v>
+        <v>0000000000010001</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
         <v>s3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -526,18 +529,18 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>00000011</v>
+        <v>0000000000011001</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
         <v>s4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -548,18 +551,18 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>00000100</v>
+        <v>0000000000100011</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
         <v>s5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -570,18 +573,18 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>00000110</v>
+        <v>0000000000101111</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
         <v>s6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -592,297 +595,297 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000000111110</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>s7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>00001000</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="3"/>
-        <v>s7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="4"/>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.62387939896722777</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000001010000</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>s8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.79369979632521837</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000001100110</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>s9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000010000000</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>s10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1.2506163847122451</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000010100000</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>s11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1.5550686885269773</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>199</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000011000111</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>s12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1.9249216229411636</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>246</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000011110110</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>s13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>2.3742241618965756</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>304</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000100110000</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>s14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2.9200431962420215</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>374</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000101110110</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>s15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>3.5831118246687113</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>459</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000111001011</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>s16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4.3886169066431755</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>562</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>0000001000110010</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>s17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>5.3671557927705953</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>687</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>0000001010101111</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>s18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>6.5558985742765259</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>839</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>0000001101000111</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>s19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>0.62387939896722777</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="2"/>
-        <v>00001010</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="3"/>
-        <v>s8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>0.79369979632521837</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="2"/>
-        <v>00001101</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="3"/>
-        <v>s9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>00010000</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="3"/>
-        <v>s10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1.2506163847122451</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>00010100</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="3"/>
-        <v>s11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1.5550686885269773</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="2"/>
-        <v>00011001</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="3"/>
-        <v>s12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1.9249216229411636</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>00011111</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="3"/>
-        <v>s13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>2.3742241618965756</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>00100110</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="3"/>
-        <v>s14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>2.9200431962420215</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="2"/>
-        <v>00101111</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="3"/>
-        <v>s15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>3.5831118246687113</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>00111001</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="3"/>
-        <v>s16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>4.3886169066431755</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>01000110</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="3"/>
-        <v>s17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>5.3671557927705953</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="2"/>
-        <v>01010110</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="3"/>
-        <v>s18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>6.5558985742765259</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="2"/>
-        <v>01101001</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="3"/>
-        <v>s19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>1024</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
-        <v>10000000</v>
+        <v>0000010000000000</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="3"/>

</xml_diff>